<commit_message>
Made some of the changes in the excel data sheet and other files
</commit_message>
<xml_diff>
--- a/MarsCompetitiveTask/MarsCompetitiveTask/ExcelData/TestExcelData.xlsx
+++ b/MarsCompetitiveTask/MarsCompetitiveTask/ExcelData/TestExcelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Other Stuff\Programming_Languages\AutomationTesting\AllProjects\ProjectMars\MarsCompetitiveTask\MarsCompetitiveTask\MarsCompetitiveTask\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE5213E-6474-4F95-953C-0835FD6A8476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E900E5-1FF9-4D41-A572-883C42FFD99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="98">
   <si>
     <t>username</t>
   </si>
@@ -307,6 +307,18 @@
   </si>
   <si>
     <t>Appium</t>
+  </si>
+  <si>
+    <t>Galaxy Test Inspector#</t>
+  </si>
+  <si>
+    <t>Software and Hardware Testing^</t>
+  </si>
+  <si>
+    <t>Jmeter</t>
+  </si>
+  <si>
+    <t>Performance Testing</t>
   </si>
 </sst>
 </file>
@@ -1667,7 +1679,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1922,6 +1936,32 @@
       </c>
       <c r="S4" s="11" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="12">
+        <v>44581</v>
+      </c>
+      <c r="M5" s="12">
+        <v>44946</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>